<commit_message>
Alterações de erros nos arquios
</commit_message>
<xml_diff>
--- a/Orçamento Infra-SystemMade.xlsx
+++ b/Orçamento Infra-SystemMade.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Igorh\Documents\MeusProjetos\InfraEstrutura-SystemMade\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E28AB22D-6D89-4E98-8057-4A836ADECA10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AA49A6C-3022-4141-A945-F93FD5F25081}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4384818C-EBB1-43CF-BA01-022AC3DC4C31}"/>
   </bookViews>
@@ -454,7 +454,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -475,12 +475,6 @@
       <color theme="1"/>
       <name val="Aharoni"/>
       <charset val="177"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -534,12 +528,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -552,8 +540,14 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -968,7 +962,7 @@
   <dimension ref="B2:K58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -999,343 +993,343 @@
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="5">
         <v>1</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="6">
         <v>1007.54</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="6">
         <f>D3*E3</f>
         <v>1007.54</v>
       </c>
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="5">
         <v>5</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="6">
         <v>1529.15</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="6">
         <f>D4*E4</f>
         <v>7645.75</v>
       </c>
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="5">
         <v>6</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="6">
         <v>379.9</v>
       </c>
-      <c r="F5" s="8">
-        <f t="shared" ref="F5:F23" si="0">D5*E5</f>
+      <c r="F5" s="6">
+        <f t="shared" ref="F5:F18" si="0">D5*E5</f>
         <v>2279.3999999999996</v>
       </c>
       <c r="G5" s="1"/>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="5">
         <v>1</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="6">
         <v>889</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="6">
         <f t="shared" si="0"/>
         <v>889</v>
       </c>
       <c r="G6" s="1"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="5">
         <v>1</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="6">
         <v>5036.8999999999996</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="6">
         <f t="shared" si="0"/>
         <v>5036.8999999999996</v>
       </c>
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="5">
         <v>6</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="6">
         <v>78.84</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="6">
         <f t="shared" si="0"/>
         <v>473.04</v>
       </c>
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="5">
         <v>1</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="6">
         <v>230</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F9" s="6">
         <f t="shared" si="0"/>
         <v>230</v>
       </c>
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="5">
         <v>3</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="6">
         <v>346.9</v>
       </c>
-      <c r="F10" s="8">
+      <c r="F10" s="6">
         <f t="shared" si="0"/>
         <v>1040.6999999999998</v>
       </c>
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="5">
         <v>1</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E11" s="6">
         <v>366.28</v>
       </c>
-      <c r="F11" s="8">
+      <c r="F11" s="6">
         <f t="shared" si="0"/>
         <v>366.28</v>
       </c>
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="5">
         <v>1</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E12" s="6">
         <v>1499</v>
       </c>
-      <c r="F12" s="8">
+      <c r="F12" s="6">
         <f t="shared" si="0"/>
         <v>1499</v>
       </c>
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="5">
         <v>1</v>
       </c>
-      <c r="E13" s="8">
+      <c r="E13" s="6">
         <v>485.05</v>
       </c>
-      <c r="F13" s="8">
+      <c r="F13" s="6">
         <f t="shared" si="0"/>
         <v>485.05</v>
       </c>
       <c r="G13" s="1"/>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D14" s="5">
         <v>2</v>
       </c>
-      <c r="E14" s="8">
+      <c r="E14" s="6">
         <v>1179</v>
       </c>
-      <c r="F14" s="8">
+      <c r="F14" s="6">
         <f t="shared" si="0"/>
         <v>2358</v>
       </c>
       <c r="G14" s="1"/>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15" s="5">
         <v>1</v>
       </c>
-      <c r="E15" s="8">
+      <c r="E15" s="6">
         <v>1566</v>
       </c>
-      <c r="F15" s="8">
+      <c r="F15" s="6">
         <f t="shared" si="0"/>
         <v>1566</v>
       </c>
       <c r="G15" s="1"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="7">
+      <c r="D16" s="5">
         <v>2</v>
       </c>
-      <c r="E16" s="8">
+      <c r="E16" s="6">
         <v>683</v>
       </c>
-      <c r="F16" s="8">
+      <c r="F16" s="6">
         <f t="shared" si="0"/>
         <v>1366</v>
       </c>
       <c r="G16" s="1"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="5">
         <v>1</v>
       </c>
-      <c r="E17" s="8">
+      <c r="E17" s="6">
         <v>157.49</v>
       </c>
-      <c r="F17" s="8">
+      <c r="F17" s="6">
         <f t="shared" si="0"/>
         <v>157.49</v>
       </c>
       <c r="G17" s="1"/>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D18" s="7">
+      <c r="D18" s="5">
         <v>2</v>
       </c>
-      <c r="E18" s="8">
+      <c r="E18" s="6">
         <v>1599</v>
       </c>
-      <c r="F18" s="8">
+      <c r="F18" s="6">
         <f t="shared" si="0"/>
         <v>3198</v>
       </c>
       <c r="G18" s="1"/>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="7">
+      <c r="D19" s="5">
         <v>3</v>
       </c>
-      <c r="E19" s="8">
+      <c r="E19" s="6">
         <v>99.9</v>
       </c>
-      <c r="F19" s="8">
-        <f>D19*E19</f>
+      <c r="F19" s="6">
+        <f t="shared" ref="F19:F30" si="1">D19*E19</f>
         <v>299.70000000000005</v>
       </c>
       <c r="G19" s="1"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D20" s="7">
+      <c r="D20" s="5">
         <v>1</v>
       </c>
-      <c r="E20" s="8">
+      <c r="E20" s="6">
         <v>439</v>
       </c>
-      <c r="F20" s="8">
-        <f>D20*E20</f>
+      <c r="F20" s="6">
+        <f t="shared" si="1"/>
         <v>439</v>
       </c>
       <c r="G20" s="1"/>
@@ -1344,206 +1338,206 @@
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D21" s="7">
+      <c r="D21" s="5">
         <v>2</v>
       </c>
-      <c r="E21" s="8">
+      <c r="E21" s="6">
         <v>179.9</v>
       </c>
-      <c r="F21" s="8">
-        <f>D21*E21</f>
+      <c r="F21" s="6">
+        <f t="shared" si="1"/>
         <v>359.8</v>
       </c>
       <c r="G21" s="1"/>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D22" s="7">
+      <c r="D22" s="5">
+        <v>1</v>
+      </c>
+      <c r="E22" s="6">
+        <v>1349.9</v>
+      </c>
+      <c r="F22" s="6">
+        <f t="shared" si="1"/>
+        <v>1349.9</v>
+      </c>
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B23" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="5">
         <v>2</v>
       </c>
-      <c r="E22" s="8">
-        <v>1349.9</v>
-      </c>
-      <c r="F22" s="8">
-        <f>D22*E22</f>
-        <v>2699.8</v>
-      </c>
-      <c r="G22" s="1"/>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D23" s="7">
+      <c r="E23" s="6">
+        <v>169.9</v>
+      </c>
+      <c r="F23" s="6">
+        <f t="shared" si="1"/>
+        <v>339.8</v>
+      </c>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B24" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" s="5">
+        <v>2</v>
+      </c>
+      <c r="E24" s="6">
+        <v>194.8</v>
+      </c>
+      <c r="F24" s="6">
+        <f t="shared" si="1"/>
+        <v>389.6</v>
+      </c>
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B25" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" s="5">
+        <v>2</v>
+      </c>
+      <c r="E25" s="6">
+        <v>109.99</v>
+      </c>
+      <c r="F25" s="6">
+        <f t="shared" si="1"/>
+        <v>219.98</v>
+      </c>
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B26" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26" s="5">
         <v>1</v>
       </c>
-      <c r="E23" s="8">
-        <v>169.9</v>
-      </c>
-      <c r="F23" s="8">
-        <f>D23*E23</f>
-        <v>169.9</v>
-      </c>
-      <c r="G23" s="1"/>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B24" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D24" s="7">
+      <c r="E26" s="6">
+        <v>165.6</v>
+      </c>
+      <c r="F26" s="6">
+        <f t="shared" si="1"/>
+        <v>165.6</v>
+      </c>
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B27" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D27" s="5">
         <v>2</v>
       </c>
-      <c r="E24" s="8">
-        <v>194.8</v>
-      </c>
-      <c r="F24" s="8">
-        <f>D24*E24</f>
-        <v>389.6</v>
-      </c>
-      <c r="G24" s="1"/>
-    </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B25" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="D25" s="7">
-        <v>2</v>
-      </c>
-      <c r="E25" s="8">
-        <v>109.99</v>
-      </c>
-      <c r="F25" s="8">
-        <f>D25*E25</f>
-        <v>219.98</v>
-      </c>
-      <c r="G25" s="1"/>
-    </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B26" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D26" s="7">
+      <c r="E27" s="6">
+        <v>996.55</v>
+      </c>
+      <c r="F27" s="6">
+        <f t="shared" si="1"/>
+        <v>1993.1</v>
+      </c>
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B28" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D28" s="5">
+        <v>5</v>
+      </c>
+      <c r="E28" s="6">
+        <v>139.9</v>
+      </c>
+      <c r="F28" s="6">
+        <f t="shared" si="1"/>
+        <v>699.5</v>
+      </c>
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B29" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D29" s="5">
+        <v>5</v>
+      </c>
+      <c r="E29" s="6">
+        <v>119.99</v>
+      </c>
+      <c r="F29" s="6">
+        <f t="shared" si="1"/>
+        <v>599.94999999999993</v>
+      </c>
+      <c r="G29" s="1"/>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B30" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D30" s="5">
         <v>1</v>
       </c>
-      <c r="E26" s="8">
-        <v>165.6</v>
-      </c>
-      <c r="F26" s="8">
-        <f>D26*E26</f>
-        <v>165.6</v>
-      </c>
-      <c r="G26" s="1"/>
-    </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B27" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="D27" s="7">
-        <v>2</v>
-      </c>
-      <c r="E27" s="8">
-        <v>996.55</v>
-      </c>
-      <c r="F27" s="8">
-        <f>D27*E27</f>
-        <v>1993.1</v>
-      </c>
-      <c r="G27" s="1"/>
-    </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B28" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D28" s="7">
-        <v>5</v>
-      </c>
-      <c r="E28" s="8">
-        <v>139.9</v>
-      </c>
-      <c r="F28" s="8">
-        <f>D28*E28</f>
-        <v>699.5</v>
-      </c>
-      <c r="G28" s="1"/>
-    </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B29" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="D29" s="7">
-        <v>5</v>
-      </c>
-      <c r="E29" s="8">
-        <v>119.99</v>
-      </c>
-      <c r="F29" s="8">
-        <f>D29*E29</f>
-        <v>599.94999999999993</v>
-      </c>
-      <c r="G29" s="1"/>
-    </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B30" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D30" s="7">
-        <v>1</v>
-      </c>
-      <c r="E30" s="8">
+      <c r="E30" s="6">
         <v>3989.9</v>
       </c>
-      <c r="F30" s="8">
-        <f>D30*E30</f>
+      <c r="F30" s="6">
+        <f t="shared" si="1"/>
         <v>3989.9</v>
       </c>
       <c r="G30" s="1"/>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="5">
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="10">
         <f>SUM(F3:F30)</f>
-        <v>41623.980000000003</v>
-      </c>
-      <c r="F31" s="5"/>
+        <v>40443.980000000003</v>
+      </c>
+      <c r="F31" s="10"/>
       <c r="G31" s="1"/>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.25">

</xml_diff>